<commit_message>
Implementar ordem de eliminação da planilha Excel - Prioridades 1-4
</commit_message>
<xml_diff>
--- a/Descricao_Comp_Rend.xlsx
+++ b/Descricao_Comp_Rend.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Composição de Rendimentos" sheetId="1" r:id="rId1"/>
     <sheet name="Regra de Aplicação" sheetId="2" r:id="rId2"/>
+    <sheet name="Ordem de Eliminação" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="118">
   <si>
     <t>CÓDIGO</t>
   </si>
@@ -359,6 +360,21 @@
   </si>
   <si>
     <t>Não</t>
+  </si>
+  <si>
+    <t>ORDEM</t>
+  </si>
+  <si>
+    <t>1 - Prioridade Máxima</t>
+  </si>
+  <si>
+    <t>3 - Facultativo Nível 3</t>
+  </si>
+  <si>
+    <t>2 - Facultativo Nível 2</t>
+  </si>
+  <si>
+    <t>4 - Analisar suspensão (Previdência | Plano de Saúde)</t>
   </si>
 </sst>
 </file>
@@ -723,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B104" sqref="B104"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J90" sqref="J90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2331,4 +2347,1053 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="49.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>217</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>3255</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>269</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>268</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>270</v>
+      </c>
+      <c r="B6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>190</v>
+      </c>
+      <c r="B7" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>266</v>
+      </c>
+      <c r="B8" t="s">
+        <v>94</v>
+      </c>
+      <c r="C8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>3193</v>
+      </c>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>3194</v>
+      </c>
+      <c r="B10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>3195</v>
+      </c>
+      <c r="B11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>3196</v>
+      </c>
+      <c r="B12" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3197</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>3198</v>
+      </c>
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>3246</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>3247</v>
+      </c>
+      <c r="B16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>15</v>
+      </c>
+      <c r="D16" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>4050</v>
+      </c>
+      <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>3169</v>
+      </c>
+      <c r="B18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>3185</v>
+      </c>
+      <c r="B19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>3186</v>
+      </c>
+      <c r="B20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>3187</v>
+      </c>
+      <c r="B21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>3188</v>
+      </c>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" t="s">
+        <v>15</v>
+      </c>
+      <c r="D22" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>3253</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>3337</v>
+      </c>
+      <c r="B24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>3338</v>
+      </c>
+      <c r="B25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C25" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>3339</v>
+      </c>
+      <c r="B26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" t="s">
+        <v>15</v>
+      </c>
+      <c r="D26" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>3235</v>
+      </c>
+      <c r="B27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>3236</v>
+      </c>
+      <c r="B28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" t="s">
+        <v>15</v>
+      </c>
+      <c r="D28" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>3237</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>3620</v>
+      </c>
+      <c r="B30" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" t="s">
+        <v>15</v>
+      </c>
+      <c r="D30" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>3621</v>
+      </c>
+      <c r="B31" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>3622</v>
+      </c>
+      <c r="B32" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>3623</v>
+      </c>
+      <c r="B33" t="s">
+        <v>104</v>
+      </c>
+      <c r="C33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3620</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+      <c r="C34" t="s">
+        <v>15</v>
+      </c>
+      <c r="D34" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>3621</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>15</v>
+      </c>
+      <c r="D35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>3622</v>
+      </c>
+      <c r="B36" t="s">
+        <v>34</v>
+      </c>
+      <c r="C36" t="s">
+        <v>15</v>
+      </c>
+      <c r="D36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>3623</v>
+      </c>
+      <c r="B37" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>3600</v>
+      </c>
+      <c r="B38" t="s">
+        <v>35</v>
+      </c>
+      <c r="C38" t="s">
+        <v>15</v>
+      </c>
+      <c r="D38" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>3601</v>
+      </c>
+      <c r="B39" t="s">
+        <v>35</v>
+      </c>
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>3221</v>
+      </c>
+      <c r="B40" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" t="s">
+        <v>15</v>
+      </c>
+      <c r="D40" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>3223</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>3330</v>
+      </c>
+      <c r="B42" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>3331</v>
+      </c>
+      <c r="B43" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>3332</v>
+      </c>
+      <c r="B44" t="s">
+        <v>38</v>
+      </c>
+      <c r="C44" t="s">
+        <v>15</v>
+      </c>
+      <c r="D44" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>3333</v>
+      </c>
+      <c r="B45" t="s">
+        <v>38</v>
+      </c>
+      <c r="C45" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>3343</v>
+      </c>
+      <c r="B46" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" t="s">
+        <v>15</v>
+      </c>
+      <c r="D46" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>3344</v>
+      </c>
+      <c r="B47" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" t="s">
+        <v>15</v>
+      </c>
+      <c r="D47" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>3345</v>
+      </c>
+      <c r="B48" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" t="s">
+        <v>15</v>
+      </c>
+      <c r="D48" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>3346</v>
+      </c>
+      <c r="B49" t="s">
+        <v>39</v>
+      </c>
+      <c r="C49" t="s">
+        <v>15</v>
+      </c>
+      <c r="D49" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>3347</v>
+      </c>
+      <c r="B50" t="s">
+        <v>39</v>
+      </c>
+      <c r="C50" t="s">
+        <v>15</v>
+      </c>
+      <c r="D50" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>3348</v>
+      </c>
+      <c r="B51" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>3280</v>
+      </c>
+      <c r="B52" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>3281</v>
+      </c>
+      <c r="B53" t="s">
+        <v>40</v>
+      </c>
+      <c r="C53" t="s">
+        <v>15</v>
+      </c>
+      <c r="D53" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>3282</v>
+      </c>
+      <c r="B54" t="s">
+        <v>40</v>
+      </c>
+      <c r="C54" t="s">
+        <v>15</v>
+      </c>
+      <c r="D54" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>3123</v>
+      </c>
+      <c r="B55" t="s">
+        <v>42</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <v>4045</v>
+      </c>
+      <c r="B56" t="s">
+        <v>43</v>
+      </c>
+      <c r="C56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D56" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <v>3167</v>
+      </c>
+      <c r="B57" t="s">
+        <v>14</v>
+      </c>
+      <c r="C57" t="s">
+        <v>15</v>
+      </c>
+      <c r="D57" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <v>3135</v>
+      </c>
+      <c r="B58" t="s">
+        <v>16</v>
+      </c>
+      <c r="C58" t="s">
+        <v>15</v>
+      </c>
+      <c r="D58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <v>3120</v>
+      </c>
+      <c r="B59" t="s">
+        <v>17</v>
+      </c>
+      <c r="C59" t="s">
+        <v>15</v>
+      </c>
+      <c r="D59" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <v>3122</v>
+      </c>
+      <c r="B60" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" t="s">
+        <v>15</v>
+      </c>
+      <c r="D60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <v>4042</v>
+      </c>
+      <c r="B61" t="s">
+        <v>95</v>
+      </c>
+      <c r="C61" t="s">
+        <v>15</v>
+      </c>
+      <c r="D61" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>278</v>
+      </c>
+      <c r="B62" t="s">
+        <v>102</v>
+      </c>
+      <c r="C62" t="s">
+        <v>15</v>
+      </c>
+      <c r="D62" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <v>278</v>
+      </c>
+      <c r="B63" t="s">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>15</v>
+      </c>
+      <c r="D63" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <v>279</v>
+      </c>
+      <c r="B64" t="s">
+        <v>24</v>
+      </c>
+      <c r="C64" t="s">
+        <v>15</v>
+      </c>
+      <c r="D64" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <v>3271</v>
+      </c>
+      <c r="B65" t="s">
+        <v>59</v>
+      </c>
+      <c r="C65" t="s">
+        <v>15</v>
+      </c>
+      <c r="D65" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>3270</v>
+      </c>
+      <c r="B66" t="s">
+        <v>60</v>
+      </c>
+      <c r="C66" t="s">
+        <v>15</v>
+      </c>
+      <c r="D66" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <v>3406</v>
+      </c>
+      <c r="B67" t="s">
+        <v>76</v>
+      </c>
+      <c r="C67" t="s">
+        <v>15</v>
+      </c>
+      <c r="D67" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <v>3405</v>
+      </c>
+      <c r="B68" t="s">
+        <v>77</v>
+      </c>
+      <c r="C68" t="s">
+        <v>15</v>
+      </c>
+      <c r="D68" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <v>3404</v>
+      </c>
+      <c r="B69" t="s">
+        <v>78</v>
+      </c>
+      <c r="C69" t="s">
+        <v>15</v>
+      </c>
+      <c r="D69" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <v>277</v>
+      </c>
+      <c r="B70" t="s">
+        <v>84</v>
+      </c>
+      <c r="C70" t="s">
+        <v>15</v>
+      </c>
+      <c r="D70" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <v>275</v>
+      </c>
+      <c r="B71" t="s">
+        <v>85</v>
+      </c>
+      <c r="C71" t="s">
+        <v>15</v>
+      </c>
+      <c r="D71" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <v>3252</v>
+      </c>
+      <c r="B72" t="s">
+        <v>96</v>
+      </c>
+      <c r="C72" t="s">
+        <v>15</v>
+      </c>
+      <c r="D72" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <v>3251</v>
+      </c>
+      <c r="B73" t="s">
+        <v>97</v>
+      </c>
+      <c r="C73" t="s">
+        <v>15</v>
+      </c>
+      <c r="D73" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:D73">
+    <sortCondition ref="D2:D73"/>
+    <sortCondition ref="B2:B73"/>
+  </sortState>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Consolidação final: 4 seções de alerta, classificação unificada, conformidade com Resolução 14/2025
</commit_message>
<xml_diff>
--- a/Descricao_Comp_Rend.xlsx
+++ b/Descricao_Comp_Rend.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210"/>
   </bookViews>
   <sheets>
     <sheet name="Composição de Rendimentos" sheetId="1" r:id="rId1"/>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C138"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J90" sqref="J90"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2353,7 +2353,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>

</xml_diff>